<commit_message>
Update Venakatesh's internship schedule.xlsx
</commit_message>
<xml_diff>
--- a/Venakatesh's internship schedule.xlsx
+++ b/Venakatesh's internship schedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="29">
   <si>
     <t>WORK SCHEDULE JAN 2025</t>
   </si>
@@ -94,7 +94,16 @@
     <t>Onbroading process</t>
   </si>
   <si>
-    <t>orientation program</t>
+    <t>Orientation program</t>
+  </si>
+  <si>
+    <t>Activity Explaination and created "DUMMY" project for the practice.</t>
+  </si>
+  <si>
+    <t>Worked with "DUMMY" project as a practice.</t>
+  </si>
+  <si>
+    <t>worked with the "DUMMY" project and completed the task as a demo.</t>
   </si>
   <si>
     <t>February</t>
@@ -120,7 +129,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +155,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -673,148 +675,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2789,8 +2791,8 @@
   <sheetPr/>
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2923,7 +2925,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" ht="72" spans="1:6">
       <c r="A9" s="7">
         <v>17</v>
       </c>
@@ -2937,8 +2939,12 @@
         <f>C9+TIME(9,0,0)</f>
         <v>0.791666666666667</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="7">
@@ -2968,7 +2974,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" ht="43.2" spans="1:6">
       <c r="A12" s="7">
         <v>20</v>
       </c>
@@ -2982,10 +2988,14 @@
         <f>C12+TIME(9,0,0)</f>
         <v>0.791666666666667</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="57.6" spans="1:6">
       <c r="A13" s="7">
         <v>21</v>
       </c>
@@ -2996,8 +3006,12 @@
         <v>12</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7">
@@ -3165,7 +3179,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="2" t="s">
@@ -3623,7 +3637,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="2" t="s">
@@ -4126,7 +4140,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B85" s="13"/>
       <c r="C85" s="2" t="s">
@@ -4360,7 +4374,7 @@
         <v>0.791666666666667</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F99" s="6"/>
     </row>

</xml_diff>